<commit_message>
Major changes to GPA Calculator
Better handled attempted credits and transfers, changed output format to
include different types of credit by course
</commit_message>
<xml_diff>
--- a/Student1Grades.xlsx
+++ b/Student1Grades.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="76">
   <si>
     <t>Course</t>
   </si>
@@ -240,6 +240,18 @@
   </si>
   <si>
     <t>Major2</t>
+  </si>
+  <si>
+    <t>Zoo699</t>
+  </si>
+  <si>
+    <t>APBio</t>
+  </si>
+  <si>
+    <t>APEngLit</t>
+  </si>
+  <si>
+    <t>APEnvSci</t>
   </si>
 </sst>
 </file>
@@ -557,10 +569,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I50"/>
+  <dimension ref="A1:I52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K26" sqref="K26"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="E49" sqref="E49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
@@ -949,7 +961,7 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21">
-        <v>2014</v>
+        <v>2015</v>
       </c>
       <c r="B21" t="s">
         <v>69</v>
@@ -1459,25 +1471,71 @@
         <v>30</v>
       </c>
     </row>
-    <row r="49" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A49">
+        <v>2012</v>
+      </c>
       <c r="B49" t="s">
         <v>65</v>
       </c>
+      <c r="C49" t="s">
+        <v>73</v>
+      </c>
       <c r="D49">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="G49" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="50" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A50">
+        <v>2012</v>
+      </c>
       <c r="B50" t="s">
         <v>65</v>
       </c>
+      <c r="C50" t="s">
+        <v>74</v>
+      </c>
       <c r="D50">
+        <v>3</v>
+      </c>
+      <c r="G50" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A51">
+        <v>2012</v>
+      </c>
+      <c r="B51" t="s">
+        <v>65</v>
+      </c>
+      <c r="C51" t="s">
+        <v>75</v>
+      </c>
+      <c r="D51">
+        <v>3</v>
+      </c>
+      <c r="G51" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A52">
+        <v>2010</v>
+      </c>
+      <c r="B52" t="s">
+        <v>65</v>
+      </c>
+      <c r="C52" t="s">
+        <v>72</v>
+      </c>
+      <c r="D52">
         <v>1</v>
       </c>
-      <c r="G50" t="s">
+      <c r="G52" t="s">
         <v>30</v>
       </c>
     </row>

</xml_diff>